<commit_message>
change nist tags for some controls
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/Documents/Projects/CMS/Inspec/STIG_Profiles/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C1BD2-4707-4423-B1B2-01297A115032}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBF945-419E-BC4D-BF6B-363BF014ED00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="480" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" r:id="rId1"/>
@@ -28162,7 +28162,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>["AC-3 (4)", "Rev_4"]</t>
+      <t>0.5</t>
     </r>
     <r>
       <rPr>
@@ -28174,50 +28174,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-AC-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
 0.0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">["IA-11", "Rev_4"]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AC-6(10)</t>
     </r>
   </si>
   <si>
@@ -28350,6 +28307,49 @@
       <t>If an emergency account must be created configure the system to
 terminate the account after a 24 hour time period with the following command to set an expiration date on it. Substitute "system_account_name" with the account to be created.
 # sudo chage -E `date -d "+1 days" +%Y-%m-%d` system_account_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">["IA-11", "Rev_4"]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>["AC-6(10)", "Rev_4"]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>["AC-3 (4)", "Rev_4"]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+["AC-3", "Rev_4"]</t>
     </r>
   </si>
 </sst>
@@ -29035,11 +29035,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
+          <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
@@ -29047,7 +29047,23 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
@@ -29365,28 +29381,28 @@
   <dimension ref="A1:AD231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.84765625" style="4"/>
-    <col min="2" max="2" width="10.84765625" style="2"/>
-    <col min="3" max="3" width="10.84765625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.6484375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="54.1484375" style="3" customWidth="1"/>
-    <col min="6" max="22" width="10.84765625" style="2" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="0.1484375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="37.1484375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="54.1640625" style="3" customWidth="1"/>
+    <col min="6" max="22" width="10.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0.1640625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="37.1640625" style="3" customWidth="1"/>
     <col min="25" max="25" width="33" style="3" customWidth="1"/>
-    <col min="26" max="27" width="10.84765625" style="2" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="15.1484375" style="3" customWidth="1"/>
-    <col min="29" max="29" width="10.1484375" style="3" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6484375" style="3" customWidth="1"/>
+    <col min="26" max="27" width="10.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="10.1640625" style="3" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="17">
       <c r="A1" s="8" t="s">
         <v>2548</v>
       </c>
@@ -29478,7 +29494,7 @@
         <v>2555</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="409.5">
+    <row r="2" spans="1:30" ht="409.6">
       <c r="A2" s="10" t="s">
         <v>1506</v>
       </c>
@@ -29544,7 +29560,7 @@
       </c>
       <c r="AD2" s="7"/>
     </row>
-    <row r="3" spans="1:30" ht="409.5">
+    <row r="3" spans="1:30" ht="409.6">
       <c r="A3" s="10" t="s">
         <v>103</v>
       </c>
@@ -29610,7 +29626,7 @@
       </c>
       <c r="AD3" s="7"/>
     </row>
-    <row r="4" spans="1:30" ht="409.5">
+    <row r="4" spans="1:30" ht="409.6">
       <c r="A4" s="12" t="s">
         <v>2341</v>
       </c>
@@ -29678,7 +29694,7 @@
       </c>
       <c r="AD4" s="11"/>
     </row>
-    <row r="5" spans="1:30" ht="409.5">
+    <row r="5" spans="1:30" ht="409.6">
       <c r="A5" s="12" t="s">
         <v>2238</v>
       </c>
@@ -29746,7 +29762,7 @@
       </c>
       <c r="AD5" s="11"/>
     </row>
-    <row r="6" spans="1:30" ht="409.5">
+    <row r="6" spans="1:30" ht="409.6">
       <c r="A6" s="10" t="s">
         <v>1042</v>
       </c>
@@ -29812,7 +29828,7 @@
       </c>
       <c r="AD6" s="7"/>
     </row>
-    <row r="7" spans="1:30" ht="409.5">
+    <row r="7" spans="1:30" ht="409.6">
       <c r="A7" s="10" t="s">
         <v>304</v>
       </c>
@@ -29880,7 +29896,7 @@
       </c>
       <c r="AD7" s="7"/>
     </row>
-    <row r="8" spans="1:30" ht="409.5">
+    <row r="8" spans="1:30" ht="409.6">
       <c r="A8" s="10" t="s">
         <v>1396</v>
       </c>
@@ -29946,7 +29962,7 @@
       </c>
       <c r="AD8" s="7"/>
     </row>
-    <row r="9" spans="1:30" ht="409.5">
+    <row r="9" spans="1:30" ht="409.6">
       <c r="A9" s="12" t="s">
         <v>619</v>
       </c>
@@ -30012,7 +30028,7 @@
       </c>
       <c r="AD9" s="7"/>
     </row>
-    <row r="10" spans="1:30" ht="409.5">
+    <row r="10" spans="1:30" ht="409.6">
       <c r="A10" s="12" t="s">
         <v>1740</v>
       </c>
@@ -30020,7 +30036,7 @@
         <v>2566</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>1736</v>
@@ -30082,7 +30098,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="409.5">
+    <row r="11" spans="1:30" ht="409.6">
       <c r="A11" s="12" t="s">
         <v>140</v>
       </c>
@@ -30148,7 +30164,7 @@
       </c>
       <c r="AD11" s="7"/>
     </row>
-    <row r="12" spans="1:30" ht="409.5">
+    <row r="12" spans="1:30" ht="409.6">
       <c r="A12" s="12" t="s">
         <v>1608</v>
       </c>
@@ -30214,7 +30230,7 @@
       </c>
       <c r="AD12" s="7"/>
     </row>
-    <row r="13" spans="1:30" ht="409.5">
+    <row r="13" spans="1:30" ht="409.6">
       <c r="A13" s="12" t="s">
         <v>844</v>
       </c>
@@ -30280,7 +30296,7 @@
       </c>
       <c r="AD13" s="7"/>
     </row>
-    <row r="14" spans="1:30" ht="409.5">
+    <row r="14" spans="1:30" ht="409.6">
       <c r="A14" s="12" t="s">
         <v>1784</v>
       </c>
@@ -30346,7 +30362,7 @@
       </c>
       <c r="AD14" s="7"/>
     </row>
-    <row r="15" spans="1:30" ht="409.5">
+    <row r="15" spans="1:30" ht="409.6">
       <c r="A15" s="12" t="s">
         <v>536</v>
       </c>
@@ -30412,7 +30428,7 @@
       </c>
       <c r="AD15" s="7"/>
     </row>
-    <row r="16" spans="1:30" ht="409.5">
+    <row r="16" spans="1:30" ht="409.6">
       <c r="A16" s="12" t="s">
         <v>178</v>
       </c>
@@ -30480,7 +30496,7 @@
       </c>
       <c r="AD16" s="11"/>
     </row>
-    <row r="17" spans="1:30" ht="409.5">
+    <row r="17" spans="1:30" ht="409.6">
       <c r="A17" s="10" t="s">
         <v>1821</v>
       </c>
@@ -30548,7 +30564,7 @@
       </c>
       <c r="AD17" s="7"/>
     </row>
-    <row r="18" spans="1:30" ht="409.5">
+    <row r="18" spans="1:30" ht="409.6">
       <c r="A18" s="10" t="s">
         <v>584</v>
       </c>
@@ -30616,7 +30632,7 @@
       </c>
       <c r="AD18" s="7"/>
     </row>
-    <row r="19" spans="1:30" ht="409.5">
+    <row r="19" spans="1:30" ht="409.6">
       <c r="A19" s="12" t="s">
         <v>1519</v>
       </c>
@@ -30682,7 +30698,7 @@
       </c>
       <c r="AD19" s="11"/>
     </row>
-    <row r="20" spans="1:30" ht="409.5">
+    <row r="20" spans="1:30" ht="409.6">
       <c r="A20" s="12" t="s">
         <v>64</v>
       </c>
@@ -30691,10 +30707,10 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>62</v>
@@ -30729,10 +30745,10 @@
       <c r="V20" s="7"/>
       <c r="W20" s="23"/>
       <c r="X20" s="22" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="Y20" s="22" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
       <c r="Z20" s="11" t="s">
         <v>70</v>
@@ -30748,7 +30764,7 @@
       </c>
       <c r="AD20" s="7"/>
     </row>
-    <row r="21" spans="1:30" ht="409.5">
+    <row r="21" spans="1:30" ht="409.6">
       <c r="A21" s="10" t="s">
         <v>1691</v>
       </c>
@@ -30814,7 +30830,7 @@
       </c>
       <c r="AD21" s="7"/>
     </row>
-    <row r="22" spans="1:30" ht="409.5">
+    <row r="22" spans="1:30" ht="409.6">
       <c r="A22" s="10" t="s">
         <v>358</v>
       </c>
@@ -30880,7 +30896,7 @@
       </c>
       <c r="AD22" s="7"/>
     </row>
-    <row r="23" spans="1:30" ht="409.5">
+    <row r="23" spans="1:30" ht="409.6">
       <c r="A23" s="12" t="s">
         <v>1495</v>
       </c>
@@ -30946,7 +30962,7 @@
       </c>
       <c r="AD23" s="7"/>
     </row>
-    <row r="24" spans="1:30" ht="409.5">
+    <row r="24" spans="1:30" ht="409.6">
       <c r="A24" s="10" t="s">
         <v>690</v>
       </c>
@@ -31012,7 +31028,7 @@
       </c>
       <c r="AD24" s="7"/>
     </row>
-    <row r="25" spans="1:30" ht="409.5">
+    <row r="25" spans="1:30" ht="409.6">
       <c r="A25" s="10" t="s">
         <v>54</v>
       </c>
@@ -31078,7 +31094,7 @@
       </c>
       <c r="AD25" s="7"/>
     </row>
-    <row r="26" spans="1:30" ht="409.5">
+    <row r="26" spans="1:30" ht="409.6">
       <c r="A26" s="10" t="s">
         <v>1131</v>
       </c>
@@ -31144,7 +31160,7 @@
       </c>
       <c r="AD26" s="7"/>
     </row>
-    <row r="27" spans="1:30" ht="409.5">
+    <row r="27" spans="1:30" ht="409.6">
       <c r="A27" s="10" t="s">
         <v>1910</v>
       </c>
@@ -31210,7 +31226,7 @@
       </c>
       <c r="AD27" s="7"/>
     </row>
-    <row r="28" spans="1:30" ht="409.5">
+    <row r="28" spans="1:30" ht="409.6">
       <c r="A28" s="12" t="s">
         <v>978</v>
       </c>
@@ -31276,7 +31292,7 @@
       </c>
       <c r="AD28" s="7"/>
     </row>
-    <row r="29" spans="1:30" ht="409.5">
+    <row r="29" spans="1:30" ht="409.6">
       <c r="A29" s="10" t="s">
         <v>2184</v>
       </c>
@@ -31344,7 +31360,7 @@
       </c>
       <c r="AD29" s="7"/>
     </row>
-    <row r="30" spans="1:30" ht="409.5">
+    <row r="30" spans="1:30" ht="409.6">
       <c r="A30" s="12" t="s">
         <v>2451</v>
       </c>
@@ -31407,7 +31423,7 @@
         <v>2459</v>
       </c>
       <c r="AB30" s="22" t="s">
-        <v>2650</v>
+        <v>2653</v>
       </c>
       <c r="AC30" s="11" t="s">
         <v>2455</v>
@@ -31416,7 +31432,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="409.5">
+    <row r="31" spans="1:30" ht="409.6">
       <c r="A31" s="12" t="s">
         <v>1334</v>
       </c>
@@ -31482,7 +31498,7 @@
       </c>
       <c r="AD31" s="7"/>
     </row>
-    <row r="32" spans="1:30" ht="409.5">
+    <row r="32" spans="1:30" ht="409.6">
       <c r="A32" s="10" t="s">
         <v>2090</v>
       </c>
@@ -31548,7 +31564,7 @@
       </c>
       <c r="AD32" s="7"/>
     </row>
-    <row r="33" spans="1:30" ht="409.5">
+    <row r="33" spans="1:30" ht="409.6">
       <c r="A33" s="10" t="s">
         <v>1013</v>
       </c>
@@ -31614,7 +31630,7 @@
       </c>
       <c r="AD33" s="7"/>
     </row>
-    <row r="34" spans="1:30" ht="409.5">
+    <row r="34" spans="1:30" ht="409.6">
       <c r="A34" s="10" t="s">
         <v>2283</v>
       </c>
@@ -31680,7 +31696,7 @@
       </c>
       <c r="AD34" s="7"/>
     </row>
-    <row r="35" spans="1:30" ht="409.5">
+    <row r="35" spans="1:30" ht="409.6">
       <c r="A35" s="10" t="s">
         <v>2463</v>
       </c>
@@ -31746,7 +31762,7 @@
       </c>
       <c r="AD35" s="7"/>
     </row>
-    <row r="36" spans="1:30" ht="409.5">
+    <row r="36" spans="1:30" ht="409.6">
       <c r="A36" s="10" t="s">
         <v>1409</v>
       </c>
@@ -31812,7 +31828,7 @@
       </c>
       <c r="AD36" s="7"/>
     </row>
-    <row r="37" spans="1:30" ht="409.5">
+    <row r="37" spans="1:30" ht="409.6">
       <c r="A37" s="10" t="s">
         <v>632</v>
       </c>
@@ -31880,7 +31896,7 @@
       </c>
       <c r="AD37" s="7"/>
     </row>
-    <row r="38" spans="1:30" ht="409.5">
+    <row r="38" spans="1:30" ht="409.6">
       <c r="A38" s="12" t="s">
         <v>1751</v>
       </c>
@@ -31946,7 +31962,7 @@
       </c>
       <c r="AD38" s="7"/>
     </row>
-    <row r="39" spans="1:30" ht="409.5">
+    <row r="39" spans="1:30" ht="409.6">
       <c r="A39" s="12" t="s">
         <v>418</v>
       </c>
@@ -32012,7 +32028,7 @@
       </c>
       <c r="AD39" s="7"/>
     </row>
-    <row r="40" spans="1:30" ht="409.5">
+    <row r="40" spans="1:30" ht="409.6">
       <c r="A40" s="10" t="s">
         <v>153</v>
       </c>
@@ -32080,7 +32096,7 @@
       </c>
       <c r="AD40" s="7"/>
     </row>
-    <row r="41" spans="1:30" ht="409.5">
+    <row r="41" spans="1:30" ht="409.6">
       <c r="A41" s="12" t="s">
         <v>1599</v>
       </c>
@@ -32146,7 +32162,7 @@
       </c>
       <c r="AD41" s="11"/>
     </row>
-    <row r="42" spans="1:30" ht="409.5">
+    <row r="42" spans="1:30" ht="409.6">
       <c r="A42" s="10" t="s">
         <v>833</v>
       </c>
@@ -32212,7 +32228,7 @@
       </c>
       <c r="AD42" s="7"/>
     </row>
-    <row r="43" spans="1:30" ht="409.5">
+    <row r="43" spans="1:30" ht="409.6">
       <c r="A43" s="10" t="s">
         <v>1771</v>
       </c>
@@ -32278,7 +32294,7 @@
       </c>
       <c r="AD43" s="7"/>
     </row>
-    <row r="44" spans="1:30" ht="409.5">
+    <row r="44" spans="1:30" ht="409.6">
       <c r="A44" s="10" t="s">
         <v>524</v>
       </c>
@@ -32344,7 +32360,7 @@
       </c>
       <c r="AD44" s="7"/>
     </row>
-    <row r="45" spans="1:30" ht="409.5">
+    <row r="45" spans="1:30" ht="409.6">
       <c r="A45" s="10" t="s">
         <v>166</v>
       </c>
@@ -32410,7 +32426,7 @@
       </c>
       <c r="AD45" s="7"/>
     </row>
-    <row r="46" spans="1:30" ht="409.5">
+    <row r="46" spans="1:30" ht="409.6">
       <c r="A46" s="10" t="s">
         <v>1832</v>
       </c>
@@ -32476,7 +32492,7 @@
       </c>
       <c r="AD46" s="7"/>
     </row>
-    <row r="47" spans="1:30" ht="409.5">
+    <row r="47" spans="1:30" ht="409.6">
       <c r="A47" s="10" t="s">
         <v>597</v>
       </c>
@@ -32546,7 +32562,7 @@
       </c>
       <c r="AD47" s="14"/>
     </row>
-    <row r="48" spans="1:30" ht="409.5">
+    <row r="48" spans="1:30" ht="409.6">
       <c r="A48" s="10" t="s">
         <v>1532</v>
       </c>
@@ -32612,7 +32628,7 @@
       </c>
       <c r="AD48" s="7"/>
     </row>
-    <row r="49" spans="1:30" ht="409.5">
+    <row r="49" spans="1:30" ht="409.6">
       <c r="A49" s="12" t="s">
         <v>797</v>
       </c>
@@ -32678,7 +32694,7 @@
       </c>
       <c r="AD49" s="11"/>
     </row>
-    <row r="50" spans="1:30" ht="409.5">
+    <row r="50" spans="1:30" ht="409.6">
       <c r="A50" s="12" t="s">
         <v>76</v>
       </c>
@@ -32686,7 +32702,7 @@
         <v>2566</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>72</v>
@@ -32748,7 +32764,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="51" spans="1:30" ht="409.5">
+    <row r="51" spans="1:30" ht="409.6">
       <c r="A51" s="10" t="s">
         <v>1677</v>
       </c>
@@ -32814,7 +32830,7 @@
       </c>
       <c r="AD51" s="7"/>
     </row>
-    <row r="52" spans="1:30" ht="409.5">
+    <row r="52" spans="1:30" ht="409.6">
       <c r="A52" s="10" t="s">
         <v>344</v>
       </c>
@@ -32882,7 +32898,7 @@
       </c>
       <c r="AD52" s="7"/>
     </row>
-    <row r="53" spans="1:30" ht="409.5">
+    <row r="53" spans="1:30" ht="409.6">
       <c r="A53" s="10" t="s">
         <v>1482</v>
       </c>
@@ -32952,7 +32968,7 @@
       </c>
       <c r="AD53" s="14"/>
     </row>
-    <row r="54" spans="1:30" ht="409.5">
+    <row r="54" spans="1:30" ht="409.6">
       <c r="A54" s="10" t="s">
         <v>676</v>
       </c>
@@ -33020,7 +33036,7 @@
       </c>
       <c r="AD54" s="7"/>
     </row>
-    <row r="55" spans="1:30" ht="409.5">
+    <row r="55" spans="1:30" ht="409.6">
       <c r="A55" s="10" t="s">
         <v>2304</v>
       </c>
@@ -33086,7 +33102,7 @@
       </c>
       <c r="AD55" s="7"/>
     </row>
-    <row r="56" spans="1:30" ht="409.5">
+    <row r="56" spans="1:30" ht="409.6">
       <c r="A56" s="10" t="s">
         <v>1097</v>
       </c>
@@ -33152,7 +33168,7 @@
       </c>
       <c r="AD56" s="7"/>
     </row>
-    <row r="57" spans="1:30" ht="409.5">
+    <row r="57" spans="1:30" ht="409.6">
       <c r="A57" s="10" t="s">
         <v>2009</v>
       </c>
@@ -33218,7 +33234,7 @@
       </c>
       <c r="AD57" s="7"/>
     </row>
-    <row r="58" spans="1:30" ht="409.5">
+    <row r="58" spans="1:30" ht="409.6">
       <c r="A58" s="10" t="s">
         <v>1284</v>
       </c>
@@ -33286,7 +33302,7 @@
       </c>
       <c r="AD58" s="7"/>
     </row>
-    <row r="59" spans="1:30" ht="409.5">
+    <row r="59" spans="1:30" ht="409.6">
       <c r="A59" s="10" t="s">
         <v>266</v>
       </c>
@@ -33352,7 +33368,7 @@
       </c>
       <c r="AD59" s="7"/>
     </row>
-    <row r="60" spans="1:30" ht="409.5">
+    <row r="60" spans="1:30" ht="409.6">
       <c r="A60" s="10" t="s">
         <v>2169</v>
       </c>
@@ -33418,7 +33434,7 @@
       </c>
       <c r="AD60" s="18"/>
     </row>
-    <row r="61" spans="1:30" ht="409.5">
+    <row r="61" spans="1:30" ht="409.6">
       <c r="A61" s="12" t="s">
         <v>873</v>
       </c>
@@ -33426,7 +33442,7 @@
         <v>2566</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>869</v>
@@ -33549,7 +33565,7 @@
         <v>1976</v>
       </c>
       <c r="AB62" s="17" t="s">
-        <v>2648</v>
+        <v>2654</v>
       </c>
       <c r="AC62" s="11" t="s">
         <v>1201</v>
@@ -33619,7 +33635,7 @@
         <v>1205</v>
       </c>
       <c r="AB63" s="17" t="s">
-        <v>2648</v>
+        <v>2654</v>
       </c>
       <c r="AC63" s="11" t="s">
         <v>1201</v>
@@ -33628,7 +33644,7 @@
         <v>2596</v>
       </c>
     </row>
-    <row r="64" spans="1:30" ht="409.5">
+    <row r="64" spans="1:30" ht="409.6">
       <c r="A64" s="10" t="s">
         <v>229</v>
       </c>
@@ -33694,7 +33710,7 @@
       </c>
       <c r="AD64" s="7"/>
     </row>
-    <row r="65" spans="1:30" ht="409.5">
+    <row r="65" spans="1:30" ht="409.6">
       <c r="A65" s="10" t="s">
         <v>1919</v>
       </c>
@@ -33760,7 +33776,7 @@
       </c>
       <c r="AD65" s="7"/>
     </row>
-    <row r="66" spans="1:30" ht="409.5">
+    <row r="66" spans="1:30" ht="409.6">
       <c r="A66" s="10" t="s">
         <v>1119</v>
       </c>
@@ -33826,7 +33842,7 @@
       </c>
       <c r="AD66" s="7"/>
     </row>
-    <row r="67" spans="1:30" ht="409.5">
+    <row r="67" spans="1:30" ht="409.6">
       <c r="A67" s="10" t="s">
         <v>2229</v>
       </c>
@@ -33892,7 +33908,7 @@
       </c>
       <c r="AD67" s="7"/>
     </row>
-    <row r="68" spans="1:30" ht="409.5">
+    <row r="68" spans="1:30" ht="409.6">
       <c r="A68" s="10" t="s">
         <v>931</v>
       </c>
@@ -33958,7 +33974,7 @@
       </c>
       <c r="AD68" s="7"/>
     </row>
-    <row r="69" spans="1:30" ht="409.5">
+    <row r="69" spans="1:30" ht="409.6">
       <c r="A69" s="10" t="s">
         <v>291</v>
       </c>
@@ -34024,7 +34040,7 @@
       </c>
       <c r="AD69" s="7"/>
     </row>
-    <row r="70" spans="1:30" ht="409.5">
+    <row r="70" spans="1:30" ht="409.6">
       <c r="A70" s="10" t="s">
         <v>2067</v>
       </c>
@@ -34090,7 +34106,7 @@
       </c>
       <c r="AD70" s="7"/>
     </row>
-    <row r="71" spans="1:30" ht="409.5">
+    <row r="71" spans="1:30" ht="409.6">
       <c r="A71" s="10" t="s">
         <v>1355</v>
       </c>
@@ -34156,7 +34172,7 @@
       </c>
       <c r="AD71" s="7"/>
     </row>
-    <row r="72" spans="1:30" ht="409.5">
+    <row r="72" spans="1:30" ht="409.6">
       <c r="A72" s="10" t="s">
         <v>2249</v>
       </c>
@@ -34222,7 +34238,7 @@
       </c>
       <c r="AD72" s="7"/>
     </row>
-    <row r="73" spans="1:30" ht="409.5">
+    <row r="73" spans="1:30" ht="409.6">
       <c r="A73" s="10" t="s">
         <v>1053</v>
       </c>
@@ -34288,7 +34304,7 @@
       </c>
       <c r="AD73" s="7"/>
     </row>
-    <row r="74" spans="1:30" ht="409.5">
+    <row r="74" spans="1:30" ht="409.6">
       <c r="A74" s="10" t="s">
         <v>317</v>
       </c>
@@ -34354,7 +34370,7 @@
       </c>
       <c r="AD74" s="7"/>
     </row>
-    <row r="75" spans="1:30" ht="409.5">
+    <row r="75" spans="1:30" ht="409.6">
       <c r="A75" s="10" t="s">
         <v>558</v>
       </c>
@@ -34420,7 +34436,7 @@
       </c>
       <c r="AD75" s="7"/>
     </row>
-    <row r="76" spans="1:30" ht="409.5">
+    <row r="76" spans="1:30" ht="409.6">
       <c r="A76" s="10" t="s">
         <v>1874</v>
       </c>
@@ -34486,7 +34502,7 @@
       </c>
       <c r="AD76" s="7"/>
     </row>
-    <row r="77" spans="1:30" ht="409.5">
+    <row r="77" spans="1:30" ht="409.6">
       <c r="A77" s="10" t="s">
         <v>786</v>
       </c>
@@ -34552,7 +34568,7 @@
       </c>
       <c r="AD77" s="7"/>
     </row>
-    <row r="78" spans="1:30" ht="409.5">
+    <row r="78" spans="1:30" ht="409.6">
       <c r="A78" s="10" t="s">
         <v>1557</v>
       </c>
@@ -34618,7 +34634,7 @@
       </c>
       <c r="AD78" s="7"/>
     </row>
-    <row r="79" spans="1:30" ht="409.5">
+    <row r="79" spans="1:30" ht="409.6">
       <c r="A79" s="10" t="s">
         <v>2411</v>
       </c>
@@ -34684,7 +34700,7 @@
       </c>
       <c r="AD79" s="7"/>
     </row>
-    <row r="80" spans="1:30" ht="409.5">
+    <row r="80" spans="1:30" ht="409.6">
       <c r="A80" s="10" t="s">
         <v>382</v>
       </c>
@@ -34750,7 +34766,7 @@
       </c>
       <c r="AD80" s="7"/>
     </row>
-    <row r="81" spans="1:30" ht="409.5">
+    <row r="81" spans="1:30" ht="409.6">
       <c r="A81" s="10" t="s">
         <v>1636</v>
       </c>
@@ -34816,7 +34832,7 @@
       </c>
       <c r="AD81" s="7"/>
     </row>
-    <row r="82" spans="1:30" ht="409.5">
+    <row r="82" spans="1:30" ht="409.6">
       <c r="A82" s="10" t="s">
         <v>712</v>
       </c>
@@ -34882,7 +34898,7 @@
       </c>
       <c r="AD82" s="7"/>
     </row>
-    <row r="83" spans="1:30" ht="409.5">
+    <row r="83" spans="1:30" ht="409.6">
       <c r="A83" s="10" t="s">
         <v>1445</v>
       </c>
@@ -34948,7 +34964,7 @@
       </c>
       <c r="AD83" s="7"/>
     </row>
-    <row r="84" spans="1:30" ht="409.5">
+    <row r="84" spans="1:30" ht="409.6">
       <c r="A84" s="10" t="s">
         <v>2366</v>
       </c>
@@ -35014,7 +35030,7 @@
       </c>
       <c r="AD84" s="7"/>
     </row>
-    <row r="85" spans="1:30" ht="409.5">
+    <row r="85" spans="1:30" ht="409.6">
       <c r="A85" s="10" t="s">
         <v>1151</v>
       </c>
@@ -35080,7 +35096,7 @@
       </c>
       <c r="AD85" s="7"/>
     </row>
-    <row r="86" spans="1:30" ht="409.5">
+    <row r="86" spans="1:30" ht="409.6">
       <c r="A86" s="10" t="s">
         <v>1883</v>
       </c>
@@ -35146,7 +35162,7 @@
       </c>
       <c r="AD86" s="7"/>
     </row>
-    <row r="87" spans="1:30" ht="409.5">
+    <row r="87" spans="1:30" ht="409.6">
       <c r="A87" s="12" t="s">
         <v>943</v>
       </c>
@@ -35154,7 +35170,7 @@
         <v>2566</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>939</v>
@@ -35216,7 +35232,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="409.5">
+    <row r="88" spans="1:30" ht="409.6">
       <c r="A88" s="12" t="s">
         <v>2209</v>
       </c>
@@ -35224,7 +35240,7 @@
         <v>2566</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>2208</v>
@@ -35286,7 +35302,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="409.5">
+    <row r="89" spans="1:30" ht="409.6">
       <c r="A89" s="12" t="s">
         <v>2429</v>
       </c>
@@ -35294,7 +35310,7 @@
         <v>2566</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>2428</v>
@@ -35356,7 +35372,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="409.5">
+    <row r="90" spans="1:30" ht="409.6">
       <c r="A90" s="12" t="s">
         <v>1324</v>
       </c>
@@ -35364,7 +35380,7 @@
         <v>2566</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>1323</v>
@@ -35426,7 +35442,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="409.5">
+    <row r="91" spans="1:30" ht="409.6">
       <c r="A91" s="12" t="s">
         <v>2108</v>
       </c>
@@ -35434,7 +35450,7 @@
         <v>2566</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D91" s="11" t="s">
         <v>2107</v>
@@ -35496,7 +35512,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="409.5">
+    <row r="92" spans="1:30" ht="409.6">
       <c r="A92" s="12" t="s">
         <v>1031</v>
       </c>
@@ -35504,7 +35520,7 @@
         <v>2566</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>1030</v>
@@ -35566,7 +35582,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="409.5">
+    <row r="93" spans="1:30" ht="409.6">
       <c r="A93" s="10" t="s">
         <v>2270</v>
       </c>
@@ -35634,7 +35650,7 @@
       </c>
       <c r="AD93" s="7"/>
     </row>
-    <row r="94" spans="1:30" ht="409.5">
+    <row r="94" spans="1:30" ht="409.6">
       <c r="A94" s="10" t="s">
         <v>1065</v>
       </c>
@@ -35700,7 +35716,7 @@
       </c>
       <c r="AD94" s="7"/>
     </row>
-    <row r="95" spans="1:30" ht="409.5">
+    <row r="95" spans="1:30" ht="409.6">
       <c r="A95" s="12" t="s">
         <v>2335</v>
       </c>
@@ -35766,7 +35782,7 @@
       </c>
       <c r="AD95" s="7"/>
     </row>
-    <row r="96" spans="1:30" ht="409.5">
+    <row r="96" spans="1:30" ht="409.6">
       <c r="A96" s="10" t="s">
         <v>1260</v>
       </c>
@@ -35832,7 +35848,7 @@
       </c>
       <c r="AD96" s="7"/>
     </row>
-    <row r="97" spans="1:30" ht="409.5">
+    <row r="97" spans="1:30" ht="409.6">
       <c r="A97" s="10" t="s">
         <v>2034</v>
       </c>
@@ -35898,7 +35914,7 @@
       </c>
       <c r="AD97" s="7"/>
     </row>
-    <row r="98" spans="1:30" ht="409.5">
+    <row r="98" spans="1:30" ht="409.6">
       <c r="A98" s="10" t="s">
         <v>2520</v>
       </c>
@@ -35964,7 +35980,7 @@
       </c>
       <c r="AD98" s="7"/>
     </row>
-    <row r="99" spans="1:30" ht="409.5">
+    <row r="99" spans="1:30" ht="409.6">
       <c r="A99" s="12" t="s">
         <v>920</v>
       </c>
@@ -35972,7 +35988,7 @@
         <v>2566</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>919</v>
@@ -36034,7 +36050,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="100" spans="1:30" ht="409.5">
+    <row r="100" spans="1:30" ht="409.6">
       <c r="A100" s="12" t="s">
         <v>2126</v>
       </c>
@@ -36042,7 +36058,7 @@
         <v>2566</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D100" s="11" t="s">
         <v>2125</v>
@@ -36104,7 +36120,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="101" spans="1:30" ht="409.5">
+    <row r="101" spans="1:30" ht="409.6">
       <c r="A101" s="10" t="s">
         <v>1216</v>
       </c>
@@ -36172,7 +36188,7 @@
       </c>
       <c r="AD101" s="7"/>
     </row>
-    <row r="102" spans="1:30" ht="409.5">
+    <row r="102" spans="1:30" ht="409.6">
       <c r="A102" s="10" t="s">
         <v>1947</v>
       </c>
@@ -36240,7 +36256,7 @@
       </c>
       <c r="AD102" s="7"/>
     </row>
-    <row r="103" spans="1:30" ht="409.5">
+    <row r="103" spans="1:30" ht="409.6">
       <c r="A103" s="10" t="s">
         <v>2511</v>
       </c>
@@ -36308,7 +36324,7 @@
       </c>
       <c r="AD103" s="7"/>
     </row>
-    <row r="104" spans="1:30" ht="409.5">
+    <row r="104" spans="1:30" ht="409.6">
       <c r="A104" s="10" t="s">
         <v>571</v>
       </c>
@@ -36376,7 +36392,7 @@
       </c>
       <c r="AD104" s="7"/>
     </row>
-    <row r="105" spans="1:30" ht="409.5">
+    <row r="105" spans="1:30" ht="409.6">
       <c r="A105" s="10" t="s">
         <v>1841</v>
       </c>
@@ -36444,7 +36460,7 @@
       </c>
       <c r="AD105" s="7"/>
     </row>
-    <row r="106" spans="1:30" ht="409.5">
+    <row r="106" spans="1:30" ht="409.6">
       <c r="A106" s="10" t="s">
         <v>759</v>
       </c>
@@ -36512,7 +36528,7 @@
       </c>
       <c r="AD106" s="7"/>
     </row>
-    <row r="107" spans="1:30" ht="409.5">
+    <row r="107" spans="1:30" ht="409.6">
       <c r="A107" s="10" t="s">
         <v>1578</v>
       </c>
@@ -36578,7 +36594,7 @@
       </c>
       <c r="AD107" s="7"/>
     </row>
-    <row r="108" spans="1:30" ht="409.5">
+    <row r="108" spans="1:30" ht="409.6">
       <c r="A108" s="10" t="s">
         <v>2402</v>
       </c>
@@ -36644,7 +36660,7 @@
       </c>
       <c r="AD108" s="7"/>
     </row>
-    <row r="109" spans="1:30" ht="409.5">
+    <row r="109" spans="1:30" ht="409.6">
       <c r="A109" s="10" t="s">
         <v>1656</v>
       </c>
@@ -36712,7 +36728,7 @@
       </c>
       <c r="AD109" s="7"/>
     </row>
-    <row r="110" spans="1:30" ht="409.5">
+    <row r="110" spans="1:30" ht="409.6">
       <c r="A110" s="10" t="s">
         <v>738</v>
       </c>
@@ -36780,7 +36796,7 @@
       </c>
       <c r="AD110" s="7"/>
     </row>
-    <row r="111" spans="1:30" ht="409.5">
+    <row r="111" spans="1:30" ht="409.6">
       <c r="A111" s="10" t="s">
         <v>1427</v>
       </c>
@@ -36848,7 +36864,7 @@
       </c>
       <c r="AD111" s="7"/>
     </row>
-    <row r="112" spans="1:30" ht="409.5">
+    <row r="112" spans="1:30" ht="409.6">
       <c r="A112" s="12" t="s">
         <v>2375</v>
       </c>
@@ -36856,7 +36872,7 @@
         <v>2566</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>2374</v>
@@ -36918,7 +36934,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="113" spans="1:30" ht="409.5">
+    <row r="113" spans="1:30" ht="409.6">
       <c r="A113" s="10" t="s">
         <v>652</v>
       </c>
@@ -36986,7 +37002,7 @@
       </c>
       <c r="AD113" s="7"/>
     </row>
-    <row r="114" spans="1:30" ht="409.5">
+    <row r="114" spans="1:30" ht="409.6">
       <c r="A114" s="10" t="s">
         <v>1384</v>
       </c>
@@ -37054,7 +37070,7 @@
       </c>
       <c r="AD114" s="7"/>
     </row>
-    <row r="115" spans="1:30" ht="409.5">
+    <row r="115" spans="1:30" ht="409.6">
       <c r="A115" s="10" t="s">
         <v>462</v>
       </c>
@@ -37122,7 +37138,7 @@
       </c>
       <c r="AD115" s="7"/>
     </row>
-    <row r="116" spans="1:30" ht="409.5">
+    <row r="116" spans="1:30" ht="409.6">
       <c r="A116" s="10" t="s">
         <v>1710</v>
       </c>
@@ -37190,7 +37206,7 @@
       </c>
       <c r="AD116" s="7"/>
     </row>
-    <row r="117" spans="1:30" ht="409.5">
+    <row r="117" spans="1:30" ht="409.6">
       <c r="A117" s="10" t="s">
         <v>1306</v>
       </c>
@@ -37258,7 +37274,7 @@
       </c>
       <c r="AD117" s="7"/>
     </row>
-    <row r="118" spans="1:30" ht="409.5">
+    <row r="118" spans="1:30" ht="409.6">
       <c r="A118" s="10" t="s">
         <v>253</v>
       </c>
@@ -37326,7 +37342,7 @@
       </c>
       <c r="AD118" s="7"/>
     </row>
-    <row r="119" spans="1:30" ht="409.5">
+    <row r="119" spans="1:30" ht="409.6">
       <c r="A119" s="10" t="s">
         <v>2148</v>
       </c>
@@ -37394,7 +37410,7 @@
       </c>
       <c r="AD119" s="7"/>
     </row>
-    <row r="120" spans="1:30" ht="409.5">
+    <row r="120" spans="1:30" ht="409.6">
       <c r="A120" s="10" t="s">
         <v>886</v>
       </c>
@@ -37462,7 +37478,7 @@
       </c>
       <c r="AD120" s="7"/>
     </row>
-    <row r="121" spans="1:30" ht="409.5">
+    <row r="121" spans="1:30" ht="409.6">
       <c r="A121" s="10" t="s">
         <v>1978</v>
       </c>
@@ -37530,7 +37546,7 @@
       </c>
       <c r="AD121" s="7"/>
     </row>
-    <row r="122" spans="1:30" ht="409.5">
+    <row r="122" spans="1:30" ht="409.6">
       <c r="A122" s="10" t="s">
         <v>1173</v>
       </c>
@@ -37598,7 +37614,7 @@
       </c>
       <c r="AD122" s="7"/>
     </row>
-    <row r="123" spans="1:30" ht="409.5">
+    <row r="123" spans="1:30" ht="409.6">
       <c r="A123" s="10" t="s">
         <v>240</v>
       </c>
@@ -37666,7 +37682,7 @@
       </c>
       <c r="AD123" s="7"/>
     </row>
-    <row r="124" spans="1:30" ht="409.5">
+    <row r="124" spans="1:30" ht="409.6">
       <c r="A124" s="10" t="s">
         <v>1566</v>
       </c>
@@ -37734,7 +37750,7 @@
       </c>
       <c r="AD124" s="7"/>
     </row>
-    <row r="125" spans="1:30" ht="409.5">
+    <row r="125" spans="1:30" ht="409.6">
       <c r="A125" s="12" t="s">
         <v>2393</v>
       </c>
@@ -37802,7 +37818,7 @@
       </c>
       <c r="AD125" s="11"/>
     </row>
-    <row r="126" spans="1:30" ht="409.5">
+    <row r="126" spans="1:30" ht="409.6">
       <c r="A126" s="12" t="s">
         <v>371</v>
       </c>
@@ -37870,7 +37886,7 @@
       </c>
       <c r="AD126" s="11"/>
     </row>
-    <row r="127" spans="1:30" ht="409.5">
+    <row r="127" spans="1:30" ht="409.6">
       <c r="A127" s="12" t="s">
         <v>1665</v>
       </c>
@@ -37938,7 +37954,7 @@
       </c>
       <c r="AD127" s="11"/>
     </row>
-    <row r="128" spans="1:30" ht="409.5">
+    <row r="128" spans="1:30" ht="409.6">
       <c r="A128" s="12" t="s">
         <v>749</v>
       </c>
@@ -38006,7 +38022,7 @@
       </c>
       <c r="AD128" s="11"/>
     </row>
-    <row r="129" spans="1:30" ht="409.5">
+    <row r="129" spans="1:30" ht="409.6">
       <c r="A129" s="12" t="s">
         <v>1436</v>
       </c>
@@ -38074,7 +38090,7 @@
       </c>
       <c r="AD129" s="11"/>
     </row>
-    <row r="130" spans="1:30" ht="409.5">
+    <row r="130" spans="1:30" ht="409.6">
       <c r="A130" s="12" t="s">
         <v>2384</v>
       </c>
@@ -38142,7 +38158,7 @@
       </c>
       <c r="AD130" s="11"/>
     </row>
-    <row r="131" spans="1:30" ht="409.5">
+    <row r="131" spans="1:30" ht="409.6">
       <c r="A131" s="12" t="s">
         <v>643</v>
       </c>
@@ -38210,7 +38226,7 @@
       </c>
       <c r="AD131" s="11"/>
     </row>
-    <row r="132" spans="1:30" ht="409.5">
+    <row r="132" spans="1:30" ht="409.6">
       <c r="A132" s="12" t="s">
         <v>1375</v>
       </c>
@@ -38278,7 +38294,7 @@
       </c>
       <c r="AD132" s="11"/>
     </row>
-    <row r="133" spans="1:30" ht="409.5">
+    <row r="133" spans="1:30" ht="409.6">
       <c r="A133" s="12" t="s">
         <v>452</v>
       </c>
@@ -38346,7 +38362,7 @@
       </c>
       <c r="AD133" s="11"/>
     </row>
-    <row r="134" spans="1:30" ht="409.5">
+    <row r="134" spans="1:30" ht="409.6">
       <c r="A134" s="12" t="s">
         <v>1701</v>
       </c>
@@ -38414,7 +38430,7 @@
       </c>
       <c r="AD134" s="11"/>
     </row>
-    <row r="135" spans="1:30" ht="409.5">
+    <row r="135" spans="1:30" ht="409.6">
       <c r="A135" s="10" t="s">
         <v>2348</v>
       </c>
@@ -38482,7 +38498,7 @@
       </c>
       <c r="AD135" s="7"/>
     </row>
-    <row r="136" spans="1:30" ht="409.5">
+    <row r="136" spans="1:30" ht="409.6">
       <c r="A136" s="10" t="s">
         <v>821</v>
       </c>
@@ -38550,7 +38566,7 @@
       </c>
       <c r="AD136" s="7"/>
     </row>
-    <row r="137" spans="1:30" ht="409.5">
+    <row r="137" spans="1:30" ht="409.6">
       <c r="A137" s="10" t="s">
         <v>1616</v>
       </c>
@@ -38618,7 +38634,7 @@
       </c>
       <c r="AD137" s="7"/>
     </row>
-    <row r="138" spans="1:30" ht="409.5">
+    <row r="138" spans="1:30" ht="409.6">
       <c r="A138" s="10" t="s">
         <v>483</v>
       </c>
@@ -38686,7 +38702,7 @@
       </c>
       <c r="AD138" s="7"/>
     </row>
-    <row r="139" spans="1:30" ht="409.5">
+    <row r="139" spans="1:30" ht="409.6">
       <c r="A139" s="10" t="s">
         <v>1812</v>
       </c>
@@ -38754,7 +38770,7 @@
       </c>
       <c r="AD139" s="7"/>
     </row>
-    <row r="140" spans="1:30" ht="409.5">
+    <row r="140" spans="1:30" ht="409.6">
       <c r="A140" s="10" t="s">
         <v>2357</v>
       </c>
@@ -38822,7 +38838,7 @@
       </c>
       <c r="AD140" s="7"/>
     </row>
-    <row r="141" spans="1:30" ht="409.5">
+    <row r="141" spans="1:30" ht="409.6">
       <c r="A141" s="10" t="s">
         <v>1160</v>
       </c>
@@ -38890,7 +38906,7 @@
       </c>
       <c r="AD141" s="7"/>
     </row>
-    <row r="142" spans="1:30" ht="409.5">
+    <row r="142" spans="1:30" ht="409.6">
       <c r="A142" s="10" t="s">
         <v>1892</v>
       </c>
@@ -38958,7 +38974,7 @@
       </c>
       <c r="AD142" s="7"/>
     </row>
-    <row r="143" spans="1:30" ht="409.5">
+    <row r="143" spans="1:30" ht="409.6">
       <c r="A143" s="10" t="s">
         <v>954</v>
       </c>
@@ -39026,7 +39042,7 @@
       </c>
       <c r="AD143" s="7"/>
     </row>
-    <row r="144" spans="1:30" ht="409.5">
+    <row r="144" spans="1:30" ht="409.6">
       <c r="A144" s="10" t="s">
         <v>2218</v>
       </c>
@@ -39094,7 +39110,7 @@
       </c>
       <c r="AD144" s="7"/>
     </row>
-    <row r="145" spans="1:30" ht="409.5">
+    <row r="145" spans="1:30" ht="409.6">
       <c r="A145" s="10" t="s">
         <v>2438</v>
       </c>
@@ -39162,7 +39178,7 @@
       </c>
       <c r="AD145" s="7"/>
     </row>
-    <row r="146" spans="1:30" ht="409.5">
+    <row r="146" spans="1:30" ht="409.6">
       <c r="A146" s="10" t="s">
         <v>1315</v>
       </c>
@@ -39230,7 +39246,7 @@
       </c>
       <c r="AD146" s="7"/>
     </row>
-    <row r="147" spans="1:30" ht="409.5">
+    <row r="147" spans="1:30" ht="409.6">
       <c r="A147" s="10" t="s">
         <v>2099</v>
       </c>
@@ -39298,7 +39314,7 @@
       </c>
       <c r="AD147" s="7"/>
     </row>
-    <row r="148" spans="1:30" ht="409.5">
+    <row r="148" spans="1:30" ht="409.6">
       <c r="A148" s="10" t="s">
         <v>1022</v>
       </c>
@@ -39366,7 +39382,7 @@
       </c>
       <c r="AD148" s="7"/>
     </row>
-    <row r="149" spans="1:30" ht="409.5">
+    <row r="149" spans="1:30" ht="409.6">
       <c r="A149" s="10" t="s">
         <v>2258</v>
       </c>
@@ -39434,7 +39450,7 @@
       </c>
       <c r="AD149" s="7"/>
     </row>
-    <row r="150" spans="1:30" ht="409.5">
+    <row r="150" spans="1:30" ht="409.6">
       <c r="A150" s="10" t="s">
         <v>2472</v>
       </c>
@@ -39502,7 +39518,7 @@
       </c>
       <c r="AD150" s="7"/>
     </row>
-    <row r="151" spans="1:30" ht="409.5">
+    <row r="151" spans="1:30" ht="409.6">
       <c r="A151" s="10" t="s">
         <v>1076</v>
       </c>
@@ -39570,7 +39586,7 @@
       </c>
       <c r="AD151" s="7"/>
     </row>
-    <row r="152" spans="1:30" ht="409.5">
+    <row r="152" spans="1:30" ht="409.6">
       <c r="A152" s="10" t="s">
         <v>1271</v>
       </c>
@@ -39638,7 +39654,7 @@
       </c>
       <c r="AD152" s="7"/>
     </row>
-    <row r="153" spans="1:30" ht="409.5">
+    <row r="153" spans="1:30" ht="409.6">
       <c r="A153" s="10" t="s">
         <v>2045</v>
       </c>
@@ -39706,7 +39722,7 @@
       </c>
       <c r="AD153" s="7"/>
     </row>
-    <row r="154" spans="1:30" ht="409.5">
+    <row r="154" spans="1:30" ht="409.6">
       <c r="A154" s="10" t="s">
         <v>2529</v>
       </c>
@@ -39774,7 +39790,7 @@
       </c>
       <c r="AD154" s="7"/>
     </row>
-    <row r="155" spans="1:30" ht="409.5">
+    <row r="155" spans="1:30" ht="409.6">
       <c r="A155" s="10" t="s">
         <v>911</v>
       </c>
@@ -39842,7 +39858,7 @@
       </c>
       <c r="AD155" s="7"/>
     </row>
-    <row r="156" spans="1:30" ht="409.5">
+    <row r="156" spans="1:30" ht="409.6">
       <c r="A156" s="10" t="s">
         <v>2117</v>
       </c>
@@ -39910,7 +39926,7 @@
       </c>
       <c r="AD156" s="7"/>
     </row>
-    <row r="157" spans="1:30" ht="409.5">
+    <row r="157" spans="1:30" ht="409.6">
       <c r="A157" s="10" t="s">
         <v>1207</v>
       </c>
@@ -39978,7 +39994,7 @@
       </c>
       <c r="AD157" s="7"/>
     </row>
-    <row r="158" spans="1:30" ht="409.5">
+    <row r="158" spans="1:30" ht="409.6">
       <c r="A158" s="10" t="s">
         <v>1938</v>
       </c>
@@ -40046,7 +40062,7 @@
       </c>
       <c r="AD158" s="7"/>
     </row>
-    <row r="159" spans="1:30" ht="409.5">
+    <row r="159" spans="1:30" ht="409.6">
       <c r="A159" s="10" t="s">
         <v>2502</v>
       </c>
@@ -40114,7 +40130,7 @@
       </c>
       <c r="AD159" s="7"/>
     </row>
-    <row r="160" spans="1:30" ht="409.5">
+    <row r="160" spans="1:30" ht="409.6">
       <c r="A160" s="10" t="s">
         <v>1418</v>
       </c>
@@ -40182,7 +40198,7 @@
       </c>
       <c r="AD160" s="7"/>
     </row>
-    <row r="161" spans="1:30" ht="409.5">
+    <row r="161" spans="1:30" ht="409.6">
       <c r="A161" s="10" t="s">
         <v>608</v>
       </c>
@@ -40250,7 +40266,7 @@
       </c>
       <c r="AD161" s="7"/>
     </row>
-    <row r="162" spans="1:30" ht="409.5">
+    <row r="162" spans="1:30" ht="409.6">
       <c r="A162" s="10" t="s">
         <v>1728</v>
       </c>
@@ -40318,7 +40334,7 @@
       </c>
       <c r="AD162" s="7"/>
     </row>
-    <row r="163" spans="1:30" ht="409.5">
+    <row r="163" spans="1:30" ht="409.6">
       <c r="A163" s="10" t="s">
         <v>431</v>
       </c>
@@ -40386,7 +40402,7 @@
       </c>
       <c r="AD163" s="7"/>
     </row>
-    <row r="164" spans="1:30" ht="409.5">
+    <row r="164" spans="1:30" ht="409.6">
       <c r="A164" s="10" t="s">
         <v>127</v>
       </c>
@@ -40454,7 +40470,7 @@
       </c>
       <c r="AD164" s="7"/>
     </row>
-    <row r="165" spans="1:30" ht="409.5">
+    <row r="165" spans="1:30" ht="409.6">
       <c r="A165" s="10" t="s">
         <v>1589</v>
       </c>
@@ -40522,7 +40538,7 @@
       </c>
       <c r="AD165" s="7"/>
     </row>
-    <row r="166" spans="1:30" ht="409.5">
+    <row r="166" spans="1:30" ht="409.6">
       <c r="A166" s="10" t="s">
         <v>852</v>
       </c>
@@ -40590,7 +40606,7 @@
       </c>
       <c r="AD166" s="7"/>
     </row>
-    <row r="167" spans="1:30" ht="409.5">
+    <row r="167" spans="1:30" ht="409.6">
       <c r="A167" s="10" t="s">
         <v>1792</v>
       </c>
@@ -40658,7 +40674,7 @@
       </c>
       <c r="AD167" s="7"/>
     </row>
-    <row r="168" spans="1:30" ht="409.5">
+    <row r="168" spans="1:30" ht="409.6">
       <c r="A168" s="10" t="s">
         <v>510</v>
       </c>
@@ -40726,7 +40742,7 @@
       </c>
       <c r="AD168" s="7"/>
     </row>
-    <row r="169" spans="1:30" ht="409.5">
+    <row r="169" spans="1:30" ht="409.6">
       <c r="A169" s="10" t="s">
         <v>192</v>
       </c>
@@ -40792,7 +40808,7 @@
       </c>
       <c r="AD169" s="7"/>
     </row>
-    <row r="170" spans="1:30" ht="409.5">
+    <row r="170" spans="1:30" ht="409.6">
       <c r="A170" s="10" t="s">
         <v>2078</v>
       </c>
@@ -40858,7 +40874,7 @@
       </c>
       <c r="AD170" s="7"/>
     </row>
-    <row r="171" spans="1:30" ht="409.5">
+    <row r="171" spans="1:30" ht="409.6">
       <c r="A171" s="12" t="s">
         <v>1343</v>
       </c>
@@ -40924,7 +40940,7 @@
       </c>
       <c r="AD171" s="11"/>
     </row>
-    <row r="172" spans="1:30" ht="409.5">
+    <row r="172" spans="1:30" ht="409.6">
       <c r="A172" s="10" t="s">
         <v>2295</v>
       </c>
@@ -40990,7 +41006,7 @@
       </c>
       <c r="AD172" s="7"/>
     </row>
-    <row r="173" spans="1:30" ht="409.5">
+    <row r="173" spans="1:30" ht="409.6">
       <c r="A173" s="12" t="s">
         <v>1000</v>
       </c>
@@ -41058,7 +41074,7 @@
       </c>
       <c r="AD173" s="11"/>
     </row>
-    <row r="174" spans="1:30" ht="409.5">
+    <row r="174" spans="1:30" ht="409.6">
       <c r="A174" s="10" t="s">
         <v>329</v>
       </c>
@@ -41124,7 +41140,7 @@
       </c>
       <c r="AD174" s="7"/>
     </row>
-    <row r="175" spans="1:30" ht="409.5">
+    <row r="175" spans="1:30" ht="409.6">
       <c r="A175" s="12" t="s">
         <v>1901</v>
       </c>
@@ -41190,7 +41206,7 @@
       </c>
       <c r="AD175" s="11"/>
     </row>
-    <row r="176" spans="1:30" ht="409.5">
+    <row r="176" spans="1:30" ht="409.6">
       <c r="A176" s="12" t="s">
         <v>1142</v>
       </c>
@@ -41256,7 +41272,7 @@
       </c>
       <c r="AD176" s="11"/>
     </row>
-    <row r="177" spans="1:30" ht="409.5">
+    <row r="177" spans="1:30" ht="409.6">
       <c r="A177" s="10" t="s">
         <v>2198</v>
       </c>
@@ -41322,7 +41338,7 @@
       </c>
       <c r="AD177" s="7"/>
     </row>
-    <row r="178" spans="1:30" ht="409.5">
+    <row r="178" spans="1:30" ht="409.6">
       <c r="A178" s="10" t="s">
         <v>966</v>
       </c>
@@ -41388,7 +41404,7 @@
       </c>
       <c r="AD178" s="7"/>
     </row>
-    <row r="179" spans="1:30" ht="409.5">
+    <row r="179" spans="1:30" ht="409.6">
       <c r="A179" s="10" t="s">
         <v>278</v>
       </c>
@@ -41454,7 +41470,7 @@
       </c>
       <c r="AD179" s="7"/>
     </row>
-    <row r="180" spans="1:30" ht="409.5">
+    <row r="180" spans="1:30" ht="409.6">
       <c r="A180" s="10" t="s">
         <v>2136</v>
       </c>
@@ -41520,7 +41536,7 @@
       </c>
       <c r="AD180" s="7"/>
     </row>
-    <row r="181" spans="1:30" ht="409.5">
+    <row r="181" spans="1:30" ht="409.6">
       <c r="A181" s="10" t="s">
         <v>899</v>
       </c>
@@ -41588,7 +41604,7 @@
       </c>
       <c r="AD181" s="7"/>
     </row>
-    <row r="182" spans="1:30" ht="409.5">
+    <row r="182" spans="1:30" ht="409.6">
       <c r="A182" s="12" t="s">
         <v>1929</v>
       </c>
@@ -41654,7 +41670,7 @@
       </c>
       <c r="AD182" s="11"/>
     </row>
-    <row r="183" spans="1:30" ht="409.5">
+    <row r="183" spans="1:30" ht="409.6">
       <c r="A183" s="10" t="s">
         <v>1227</v>
       </c>
@@ -41720,7 +41736,7 @@
       </c>
       <c r="AD183" s="7"/>
     </row>
-    <row r="184" spans="1:30" ht="409.5">
+    <row r="184" spans="1:30" ht="409.6">
       <c r="A184" s="12" t="s">
         <v>218</v>
       </c>
@@ -41786,7 +41802,7 @@
       </c>
       <c r="AD184" s="11"/>
     </row>
-    <row r="185" spans="1:30" ht="409.5">
+    <row r="185" spans="1:30" ht="409.6">
       <c r="A185" s="12" t="s">
         <v>2325</v>
       </c>
@@ -41854,7 +41870,7 @@
       </c>
       <c r="AD185" s="11"/>
     </row>
-    <row r="186" spans="1:30" ht="409.5">
+    <row r="186" spans="1:30" ht="409.6">
       <c r="A186" s="10" t="s">
         <v>1085</v>
       </c>
@@ -41920,7 +41936,7 @@
       </c>
       <c r="AD186" s="7"/>
     </row>
-    <row r="187" spans="1:30" ht="409.5">
+    <row r="187" spans="1:30" ht="409.6">
       <c r="A187" s="10" t="s">
         <v>2056</v>
       </c>
@@ -41986,7 +42002,7 @@
       </c>
       <c r="AD187" s="7"/>
     </row>
-    <row r="188" spans="1:30" ht="409.5">
+    <row r="188" spans="1:30" ht="409.6">
       <c r="A188" s="12" t="s">
         <v>1248</v>
       </c>
@@ -42052,7 +42068,7 @@
       </c>
       <c r="AD188" s="7"/>
     </row>
-    <row r="189" spans="1:30" ht="409.5">
+    <row r="189" spans="1:30" ht="409.6">
       <c r="A189" s="10" t="s">
         <v>1647</v>
       </c>
@@ -42118,7 +42134,7 @@
       </c>
       <c r="AD189" s="7"/>
     </row>
-    <row r="190" spans="1:30" ht="409.5">
+    <row r="190" spans="1:30" ht="409.6">
       <c r="A190" s="10" t="s">
         <v>407</v>
       </c>
@@ -42184,7 +42200,7 @@
       </c>
       <c r="AD190" s="7"/>
     </row>
-    <row r="191" spans="1:30" ht="409.5">
+    <row r="191" spans="1:30" ht="409.6">
       <c r="A191" s="10" t="s">
         <v>1469</v>
       </c>
@@ -42250,7 +42266,7 @@
       </c>
       <c r="AD191" s="7"/>
     </row>
-    <row r="192" spans="1:30" ht="409.5">
+    <row r="192" spans="1:30" ht="409.6">
       <c r="A192" s="10" t="s">
         <v>725</v>
       </c>
@@ -42316,7 +42332,7 @@
       </c>
       <c r="AD192" s="7"/>
     </row>
-    <row r="193" spans="1:30" ht="409.5">
+    <row r="193" spans="1:30" ht="409.6">
       <c r="A193" s="10" t="s">
         <v>41</v>
       </c>
@@ -42382,7 +42398,7 @@
       </c>
       <c r="AD193" s="7"/>
     </row>
-    <row r="194" spans="1:30" ht="409.5">
+    <row r="194" spans="1:30" ht="409.6">
       <c r="A194" s="10" t="s">
         <v>1852</v>
       </c>
@@ -42448,7 +42464,7 @@
       </c>
       <c r="AD194" s="7"/>
     </row>
-    <row r="195" spans="1:30" ht="409.5">
+    <row r="195" spans="1:30" ht="409.6">
       <c r="A195" s="10" t="s">
         <v>547</v>
       </c>
@@ -42514,7 +42530,7 @@
       </c>
       <c r="AD195" s="7"/>
     </row>
-    <row r="196" spans="1:30" ht="409.5">
+    <row r="196" spans="1:30" ht="409.6">
       <c r="A196" s="10" t="s">
         <v>1546</v>
       </c>
@@ -42580,7 +42596,7 @@
       </c>
       <c r="AD196" s="7"/>
     </row>
-    <row r="197" spans="1:30" ht="409.5">
+    <row r="197" spans="1:30" ht="409.6">
       <c r="A197" s="10" t="s">
         <v>773</v>
       </c>
@@ -42648,7 +42664,7 @@
       </c>
       <c r="AD197" s="7"/>
     </row>
-    <row r="198" spans="1:30" ht="409.5">
+    <row r="198" spans="1:30" ht="409.6">
       <c r="A198" s="12" t="s">
         <v>90</v>
       </c>
@@ -42656,7 +42672,7 @@
         <v>2566</v>
       </c>
       <c r="C198" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D198" s="11" t="s">
         <v>86</v>
@@ -42718,7 +42734,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="199" spans="1:30" ht="409.5">
+    <row r="199" spans="1:30" ht="409.6">
       <c r="A199" s="12" t="s">
         <v>810</v>
       </c>
@@ -42784,7 +42800,7 @@
       </c>
       <c r="AD199" s="11"/>
     </row>
-    <row r="200" spans="1:30" ht="409.5">
+    <row r="200" spans="1:30" ht="409.6">
       <c r="A200" s="10" t="s">
         <v>1803</v>
       </c>
@@ -42850,7 +42866,7 @@
       </c>
       <c r="AD200" s="7"/>
     </row>
-    <row r="201" spans="1:30" ht="409.5">
+    <row r="201" spans="1:30" ht="409.6">
       <c r="A201" s="12" t="s">
         <v>495</v>
       </c>
@@ -42918,7 +42934,7 @@
       </c>
       <c r="AD201" s="7"/>
     </row>
-    <row r="202" spans="1:30" ht="409.5">
+    <row r="202" spans="1:30" ht="409.6">
       <c r="A202" s="12" t="s">
         <v>206</v>
       </c>
@@ -42926,7 +42942,7 @@
         <v>2566</v>
       </c>
       <c r="C202" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D202" s="11" t="s">
         <v>202</v>
@@ -42988,7 +43004,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="203" spans="1:30" ht="409.5">
+    <row r="203" spans="1:30" ht="409.6">
       <c r="A203" s="10" t="s">
         <v>1366</v>
       </c>
@@ -43054,7 +43070,7 @@
       </c>
       <c r="AD203" s="7"/>
     </row>
-    <row r="204" spans="1:30" ht="409.5">
+    <row r="204" spans="1:30" ht="409.6">
       <c r="A204" s="10" t="s">
         <v>663</v>
       </c>
@@ -43120,7 +43136,7 @@
       </c>
       <c r="AD204" s="7"/>
     </row>
-    <row r="205" spans="1:30" ht="409.5">
+    <row r="205" spans="1:30" ht="409.6">
       <c r="A205" s="10" t="s">
         <v>1719</v>
       </c>
@@ -43186,7 +43202,7 @@
       </c>
       <c r="AD205" s="7"/>
     </row>
-    <row r="206" spans="1:30" ht="409.5">
+    <row r="206" spans="1:30" ht="409.6">
       <c r="A206" s="10" t="s">
         <v>442</v>
       </c>
@@ -43252,7 +43268,7 @@
       </c>
       <c r="AD206" s="7"/>
     </row>
-    <row r="207" spans="1:30" ht="409.5">
+    <row r="207" spans="1:30" ht="409.6">
       <c r="A207" s="10" t="s">
         <v>114</v>
       </c>
@@ -43318,7 +43334,7 @@
       </c>
       <c r="AD207" s="7"/>
     </row>
-    <row r="208" spans="1:30" ht="409.5">
+    <row r="208" spans="1:30" ht="409.6">
       <c r="A208" s="10" t="s">
         <v>861</v>
       </c>
@@ -43384,7 +43400,7 @@
       </c>
       <c r="AD208" s="7"/>
     </row>
-    <row r="209" spans="1:30" ht="409.5">
+    <row r="209" spans="1:30" ht="409.6">
       <c r="A209" s="10" t="s">
         <v>2157</v>
       </c>
@@ -43450,7 +43466,7 @@
       </c>
       <c r="AD209" s="7"/>
     </row>
-    <row r="210" spans="1:30" ht="409.5">
+    <row r="210" spans="1:30" ht="409.6">
       <c r="A210" s="10" t="s">
         <v>1186</v>
       </c>
@@ -43516,7 +43532,7 @@
       </c>
       <c r="AD210" s="7"/>
     </row>
-    <row r="211" spans="1:30" ht="409.5">
+    <row r="211" spans="1:30" ht="409.6">
       <c r="A211" s="10" t="s">
         <v>1958</v>
       </c>
@@ -43582,7 +43598,7 @@
       </c>
       <c r="AD211" s="7"/>
     </row>
-    <row r="212" spans="1:30" ht="409.5">
+    <row r="212" spans="1:30" ht="409.6">
       <c r="A212" s="10" t="s">
         <v>2493</v>
       </c>
@@ -43648,7 +43664,7 @@
       </c>
       <c r="AD212" s="7"/>
     </row>
-    <row r="213" spans="1:30" ht="409.5">
+    <row r="213" spans="1:30" ht="409.6">
       <c r="A213" s="10" t="s">
         <v>1108</v>
       </c>
@@ -43714,7 +43730,7 @@
       </c>
       <c r="AD213" s="7"/>
     </row>
-    <row r="214" spans="1:30" ht="409.5">
+    <row r="214" spans="1:30" ht="409.6">
       <c r="A214" s="10" t="s">
         <v>2313</v>
       </c>
@@ -43780,7 +43796,7 @@
       </c>
       <c r="AD214" s="7"/>
     </row>
-    <row r="215" spans="1:30" ht="409.5">
+    <row r="215" spans="1:30" ht="409.6">
       <c r="A215" s="10" t="s">
         <v>1297</v>
       </c>
@@ -43846,7 +43862,7 @@
       </c>
       <c r="AD215" s="7"/>
     </row>
-    <row r="216" spans="1:30" ht="409.5">
+    <row r="216" spans="1:30" ht="409.6">
       <c r="A216" s="10" t="s">
         <v>2020</v>
       </c>
@@ -43912,7 +43928,7 @@
       </c>
       <c r="AD216" s="7"/>
     </row>
-    <row r="217" spans="1:30" ht="409.5">
+    <row r="217" spans="1:30" ht="409.6">
       <c r="A217" s="10" t="s">
         <v>2540</v>
       </c>
@@ -43978,7 +43994,7 @@
       </c>
       <c r="AD217" s="7"/>
     </row>
-    <row r="218" spans="1:30" ht="409.5">
+    <row r="218" spans="1:30" ht="409.6">
       <c r="A218" s="10" t="s">
         <v>1627</v>
       </c>
@@ -44044,7 +44060,7 @@
       </c>
       <c r="AD218" s="7"/>
     </row>
-    <row r="219" spans="1:30" ht="409.5">
+    <row r="219" spans="1:30" ht="409.6">
       <c r="A219" s="12" t="s">
         <v>394</v>
       </c>
@@ -44112,7 +44128,7 @@
       </c>
       <c r="AD219" s="11"/>
     </row>
-    <row r="220" spans="1:30" ht="409.5">
+    <row r="220" spans="1:30" ht="409.6">
       <c r="A220" s="12" t="s">
         <v>1456</v>
       </c>
@@ -44178,7 +44194,7 @@
       </c>
       <c r="AD220" s="11"/>
     </row>
-    <row r="221" spans="1:30" ht="409.5">
+    <row r="221" spans="1:30" ht="409.6">
       <c r="A221" s="12" t="s">
         <v>700</v>
       </c>
@@ -44246,7 +44262,7 @@
       </c>
       <c r="AD221" s="11"/>
     </row>
-    <row r="222" spans="1:30" ht="409.5">
+    <row r="222" spans="1:30" ht="409.6">
       <c r="A222" s="10" t="s">
         <v>27</v>
       </c>
@@ -44314,7 +44330,7 @@
       </c>
       <c r="AD222" s="7"/>
     </row>
-    <row r="223" spans="1:30" ht="409.5">
+    <row r="223" spans="1:30" ht="409.6">
       <c r="A223" s="12" t="s">
         <v>1864</v>
       </c>
@@ -44382,7 +44398,7 @@
       </c>
       <c r="AD223" s="11"/>
     </row>
-    <row r="224" spans="1:30" ht="409.5">
+    <row r="224" spans="1:30" ht="409.6">
       <c r="A224" s="12" t="s">
         <v>1761</v>
       </c>
@@ -44448,7 +44464,7 @@
       </c>
       <c r="AD224" s="11"/>
     </row>
-    <row r="225" spans="1:30" ht="409.5">
+    <row r="225" spans="1:30" ht="409.6">
       <c r="A225" s="12" t="s">
         <v>474</v>
       </c>
@@ -44514,7 +44530,7 @@
       </c>
       <c r="AD225" s="11"/>
     </row>
-    <row r="226" spans="1:30" ht="409.5">
+    <row r="226" spans="1:30" ht="409.6">
       <c r="A226" s="10" t="s">
         <v>1989</v>
       </c>
@@ -44580,7 +44596,7 @@
       </c>
       <c r="AD226" s="7"/>
     </row>
-    <row r="227" spans="1:30" ht="409.5">
+    <row r="227" spans="1:30" ht="409.6">
       <c r="A227" s="12" t="s">
         <v>2482</v>
       </c>
@@ -44646,7 +44662,7 @@
       </c>
       <c r="AD227" s="11"/>
     </row>
-    <row r="228" spans="1:30" ht="409.5">
+    <row r="228" spans="1:30" ht="409.6">
       <c r="A228" s="12" t="s">
         <v>1237</v>
       </c>
@@ -44712,7 +44728,7 @@
       </c>
       <c r="AD228" s="7"/>
     </row>
-    <row r="229" spans="1:30" ht="409.5">
+    <row r="229" spans="1:30" ht="409.6">
       <c r="A229" s="10" t="s">
         <v>1998</v>
       </c>
@@ -44778,7 +44794,7 @@
       </c>
       <c r="AD229" s="7"/>
     </row>
-    <row r="230" spans="1:30" ht="409.5">
+    <row r="230" spans="1:30" ht="409.6">
       <c r="A230" s="12" t="s">
         <v>988</v>
       </c>
@@ -44786,7 +44802,7 @@
         <v>2566</v>
       </c>
       <c r="C230" s="17" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="D230" s="11" t="s">
         <v>986</v>
@@ -44848,7 +44864,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="231" spans="1:30" ht="409.5">
+    <row r="231" spans="1:30" ht="409.6">
       <c r="A231" s="10" t="s">
         <v>2420</v>
       </c>
@@ -44915,7 +44931,11 @@
       <c r="AD231" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD231" xr:uid="{61D0250F-7748-724D-80F5-9006D9A8483B}"/>
+  <autoFilter ref="A1:AD231" xr:uid="{61D0250F-7748-724D-80F5-9006D9A8483B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD231">
+      <sortCondition ref="A1:A231"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -44929,9 +44949,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="312">
+    <row r="1" spans="1:4" ht="356">
       <c r="A1" s="6" t="s">
         <v>2561</v>
       </c>

</xml_diff>

<commit_message>
added all changed controls to overlay.rb
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishna/Documents/Projects/CMS/Inspec/STIG_Profiles/cms-ars-3.1-high-canonical-ubuntu-16.04-lts-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBF945-419E-BC4D-BF6B-363BF014ED00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6784C516-F8F0-8C44-98B6-A37607A1F131}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="480" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" r:id="rId1"/>
@@ -23034,106 +23034,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Verify the Ubuntu operating system displays the Standard
-Mandatory </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Notice and Consent Banner before granting access to the Ubuntu
-operating system via a ssh logon.
-Check that the Ubuntu operating system displays the Standard Mandatory DoD
-Notice and Consent Banner before granting access to the Ubuntu operating system
-via a ssh logon with the following command:
-# grep -i banner /etc/ssh/sshd_config
-Banner=/etc/issue.net
-The command will return the banner option along with the name of the file that
-contains the ssh banner. If the line is commented out this is a finding.
-Check the specified banner file to check that it matches the Standard Mandatory
-DoD Notice and Consent Banner exactly:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">"* This warning banner provides privacy and security notices consistent with applicable federal laws, directives, and other federal guidance for accessing this Government system, which includes (1) this computer network, (2) all computers connected to this network, and (3) all devices and storage media attached to this network or to a computer on this network.
-* This system is provided for Government authorized use only.
-* Unauthorized or improper use of this system is prohibited and may result in disciplinary action and/or civil and criminal penalties.
-* Personal use of social media and networking sites on this system is limited as to not interfere with official work duties and is subject to monitoring.
-* By using this system, you understand and consent to the following:
-- The Government may monitor, record, and audit your system usage, including usage of personal devices and email systems for official duties or to conduct HHS business. Therefore, you have no reasonable expectation of privacy regarding any communication or data transiting or stored on this system. At any time, and for any lawful Government purpose, the government may monitor, intercept, and search and seize any communication or data transiting or stored on this system.
-- Any communication or data transiting or stored on this system may be disclosed or used for any lawful Government purpose'"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If the banner text does not match the Standard Mandatory </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Notice and Consent
-Banner exactly, this is a finding.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">(not in ARS)
 Add to Overlay:
 desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is </t>
@@ -26244,297 +26144,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> minutes of inactivity.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Verify that all network connections associated with SSH traffic
-are automatically terminated at the end of the session or after "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>30</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" minutes
-of inactivity.
-Check that the "ClientAliveInterval" variable is set to a value of "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>600</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" or
-less by performing the following command:
-# sudo grep -i clientalive /etc/ssh/sshd_config
-ClientAliveInterval </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>600</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ClientAliveCountMax  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If "ClientAliveInterval" or "ClientAliveCountMax" does not exist,
-"ClientAliveInterval" is not set to a value of "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>600</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" or less and
-"ClientAliveCountMax" is not set to a value of "1" or greater in
-"/etc/ssh/sshd_config", or either line is commented out, this is a finding.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Configure the Ubuntu operating system to automatically terminate
-all network connections associated with SSH traffic at the end of a session or
-after a "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>30</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" minute period of inactivity.
-Modify or append the following lines in the "/etc/ssh/sshd_config" file
-replacing "[Interval]" with a value of "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>600</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" or less and "[CountMax] with
-a value of "1" or greater:
-ClientAliveInterval </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>600</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ClientAliveCountMax  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-In order for the changes to take effect, the SSH daemon must be restarted.
-# sudo systemctl restart sshd.service</t>
     </r>
   </si>
   <si>
@@ -28350,6 +27959,551 @@
       </rPr>
       <t xml:space="preserve">
 ["AC-3", "Rev_4"]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify that all network connections associated with SSH traffic
+are automatically terminated at the end of the session or after "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" minutes
+of inactivity.
+Check that the "ClientAliveInterval" variable is set to a value of "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" or
+less by performing the following command:
+# sudo grep -i clientalive /etc/ssh/sshd_config
+ClientAliveInterval </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ClientAliveCountMax  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If "ClientAliveInterval" or "ClientAliveCountMax" does not exist,
+"ClientAliveInterval" is not set to a value of "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" or less and
+"ClientAliveCountMax" is not set to a value of "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>or greater</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in
+"/etc/ssh/sshd_config", or either line is commented out, this is a finding.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Configure the Ubuntu operating system to automatically terminate
+all network connections associated with SSH traffic at the end of a session or
+after a "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" minute period of inactivity.
+Modify or append the following lines in the "/etc/ssh/sshd_config" file
+replacing "[Interval]" with a value of "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" or less and "[CountMax] with
+a value of "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>or greater</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ClientAliveInterval </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ClientAliveCountMax  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+In order for the changes to take effect, the SSH daemon must be restarted.
+# sudo systemctl restart sshd.service</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify the Ubuntu operating system displays the Standard
+Mandatory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Notice and Consent Banner before granting access to the Ubuntu
+operating system via a ssh logon.
+Check that the Ubuntu operating system displays the Standard Mandatory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Notice and Consent Banner before granting access to the Ubuntu operating system
+via a ssh logon with the following command:
+# grep -i banner /etc/ssh/sshd_config
+Banner=/etc/issue.net
+The command will return the banner option along with the name of the file that
+contains the ssh banner. If the line is commented out this is a finding.
+Check the specified banner file to check that it matches the Standard Mandatory
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Notice and Consent Banner exactly:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">"* This warning banner provides privacy and security notices consistent with applicable federal laws, directives, and other federal guidance for accessing this Government system, which includes (1) this computer network, (2) all computers connected to this network, and (3) all devices and storage media attached to this network or to a computer on this network.
+* This system is provided for Government authorized use only.
+* Unauthorized or improper use of this system is prohibited and may result in disciplinary action and/or civil and criminal penalties.
+* Personal use of social media and networking sites on this system is limited as to not interfere with official work duties and is subject to monitoring.
+* By using this system, you understand and consent to the following:
+- The Government may monitor, record, and audit your system usage, including usage of personal devices and email systems for official duties or to conduct HHS business. Therefore, you have no reasonable expectation of privacy regarding any communication or data transiting or stored on this system. At any time, and for any lawful Government purpose, the government may monitor, intercept, and search and seize any communication or data transiting or stored on this system.
+- Any communication or data transiting or stored on this system may be disclosed or used for any lawful Government purpose'"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If the banner text does not match the Standard Mandatory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Notice and Consent
+Banner exactly, this is a finding.</t>
     </r>
   </si>
 </sst>
@@ -29035,40 +29189,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -29382,7 +29503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB25" sqref="AB25"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -29635,10 +29756,10 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>1927</v>
@@ -29678,7 +29799,7 @@
         <v>107</v>
       </c>
       <c r="Y4" s="20" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="Z4" s="11" t="s">
         <v>2345</v>
@@ -29703,10 +29824,10 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>1927</v>
@@ -29743,10 +29864,10 @@
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
       <c r="X5" s="20" t="s">
+        <v>2590</v>
+      </c>
+      <c r="Y5" s="20" t="s">
         <v>2591</v>
-      </c>
-      <c r="Y5" s="20" t="s">
-        <v>2592</v>
       </c>
       <c r="Z5" s="11" t="s">
         <v>2244</v>
@@ -29971,7 +30092,7 @@
         <v>0.3</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>2628</v>
+        <v>2625</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>616</v>
@@ -30009,10 +30130,10 @@
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="20" t="s">
-        <v>2629</v>
+        <v>2626</v>
       </c>
       <c r="Y9" s="20" t="s">
-        <v>2630</v>
+        <v>2627</v>
       </c>
       <c r="Z9" s="11" t="s">
         <v>625</v>
@@ -30033,10 +30154,10 @@
         <v>1740</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>1736</v>
@@ -30107,7 +30228,7 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>137</v>
@@ -30145,10 +30266,10 @@
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
       <c r="X11" s="20" t="s">
+        <v>2598</v>
+      </c>
+      <c r="Y11" s="20" t="s">
         <v>2599</v>
-      </c>
-      <c r="Y11" s="20" t="s">
-        <v>2600</v>
       </c>
       <c r="Z11" s="11" t="s">
         <v>146</v>
@@ -30173,7 +30294,7 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>137</v>
@@ -30211,10 +30332,10 @@
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
       <c r="X12" s="20" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="Y12" s="20" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="Z12" s="11" t="s">
         <v>1613</v>
@@ -30239,7 +30360,7 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>137</v>
@@ -30277,10 +30398,10 @@
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="20" t="s">
+        <v>2604</v>
+      </c>
+      <c r="Y13" s="20" t="s">
         <v>2605</v>
-      </c>
-      <c r="Y13" s="20" t="s">
-        <v>2606</v>
       </c>
       <c r="Z13" s="11" t="s">
         <v>849</v>
@@ -30305,7 +30426,7 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>1781</v>
@@ -30343,10 +30464,10 @@
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
       <c r="X14" s="20" t="s">
+        <v>2607</v>
+      </c>
+      <c r="Y14" s="20" t="s">
         <v>2608</v>
-      </c>
-      <c r="Y14" s="20" t="s">
-        <v>2609</v>
       </c>
       <c r="Z14" s="11" t="s">
         <v>1789</v>
@@ -30371,10 +30492,10 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="20" t="s">
+        <v>2609</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>2610</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>2611</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>534</v>
@@ -30409,10 +30530,10 @@
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
       <c r="X15" s="20" t="s">
+        <v>2611</v>
+      </c>
+      <c r="Y15" s="20" t="s">
         <v>2612</v>
-      </c>
-      <c r="Y15" s="20" t="s">
-        <v>2613</v>
       </c>
       <c r="Z15" s="11" t="s">
         <v>542</v>
@@ -30440,7 +30561,7 @@
         <v>174</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>175</v>
@@ -30644,7 +30765,7 @@
         <v>1516</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>1517</v>
@@ -30682,7 +30803,7 @@
         <v>1525</v>
       </c>
       <c r="Y19" s="20" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="Z19" s="11" t="s">
         <v>1526</v>
@@ -30707,10 +30828,10 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>2649</v>
+        <v>2646</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>2650</v>
+        <v>2647</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>62</v>
@@ -30745,10 +30866,10 @@
       <c r="V20" s="7"/>
       <c r="W20" s="23"/>
       <c r="X20" s="22" t="s">
-        <v>2651</v>
+        <v>2648</v>
       </c>
       <c r="Y20" s="22" t="s">
-        <v>2652</v>
+        <v>2649</v>
       </c>
       <c r="Z20" s="11" t="s">
         <v>70</v>
@@ -30905,7 +31026,7 @@
         <v>0.5</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>1492</v>
@@ -30943,10 +31064,10 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="20" t="s">
+        <v>2614</v>
+      </c>
+      <c r="Y23" s="20" t="s">
         <v>2615</v>
-      </c>
-      <c r="Y23" s="20" t="s">
-        <v>2616</v>
       </c>
       <c r="Z23" s="11" t="s">
         <v>1501</v>
@@ -31235,10 +31356,10 @@
         <v>0.5</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>2624</v>
+        <v>2621</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>2625</v>
+        <v>2622</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>976</v>
@@ -31273,10 +31394,10 @@
       <c r="V28" s="7"/>
       <c r="W28" s="21"/>
       <c r="X28" s="20" t="s">
-        <v>2626</v>
+        <v>2623</v>
       </c>
       <c r="Y28" s="20" t="s">
-        <v>2627</v>
+        <v>2624</v>
       </c>
       <c r="Z28" s="11" t="s">
         <v>984</v>
@@ -31365,7 +31486,7 @@
         <v>2451</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C30" s="7">
         <v>0.5</v>
@@ -31423,13 +31544,13 @@
         <v>2459</v>
       </c>
       <c r="AB30" s="22" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="AC30" s="11" t="s">
         <v>2455</v>
       </c>
       <c r="AD30" s="15" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="409.6">
@@ -31441,10 +31562,10 @@
         <v>0.5</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>2647</v>
+        <v>2644</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>2621</v>
+        <v>2618</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>1332</v>
@@ -31479,10 +31600,10 @@
       <c r="V31" s="21"/>
       <c r="W31" s="21"/>
       <c r="X31" s="20" t="s">
-        <v>2622</v>
+        <v>2619</v>
       </c>
       <c r="Y31" s="20" t="s">
-        <v>2623</v>
+        <v>2620</v>
       </c>
       <c r="Z31" s="11" t="s">
         <v>1339</v>
@@ -31908,7 +32029,7 @@
         <v>1750</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>2638</v>
+        <v>2635</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>416</v>
@@ -31974,7 +32095,7 @@
         <v>415</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>2638</v>
+        <v>2635</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>416</v>
@@ -32108,7 +32229,7 @@
         <v>1597</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>1598</v>
@@ -32497,7 +32618,7 @@
         <v>597</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C47" s="7">
         <v>0.5</v>
@@ -32640,7 +32761,7 @@
         <v>794</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>795</v>
@@ -32699,10 +32820,10 @@
         <v>76</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>72</v>
@@ -32903,7 +33024,7 @@
         <v>1482</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C53" s="7">
         <v>0.5</v>
@@ -33439,10 +33560,10 @@
         <v>873</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>869</v>
@@ -33509,7 +33630,7 @@
         <v>1969</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C62" s="7">
         <v>0.5</v>
@@ -33565,13 +33686,13 @@
         <v>1976</v>
       </c>
       <c r="AB62" s="17" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="AC62" s="11" t="s">
         <v>1201</v>
       </c>
       <c r="AD62" s="15" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="263.5" customHeight="1">
@@ -33579,7 +33700,7 @@
         <v>1197</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C63" s="7">
         <v>0.5</v>
@@ -33635,13 +33756,13 @@
         <v>1205</v>
       </c>
       <c r="AB63" s="17" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="AC63" s="11" t="s">
         <v>1201</v>
       </c>
       <c r="AD63" s="15" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="64" spans="1:30" ht="409.6">
@@ -35167,10 +35288,10 @@
         <v>943</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>939</v>
@@ -35237,10 +35358,10 @@
         <v>2209</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>2208</v>
@@ -35307,10 +35428,10 @@
         <v>2429</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>2428</v>
@@ -35377,10 +35498,10 @@
         <v>1324</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>1323</v>
@@ -35447,10 +35568,10 @@
         <v>2108</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D91" s="11" t="s">
         <v>2107</v>
@@ -35517,10 +35638,10 @@
         <v>1031</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>1030</v>
@@ -35725,10 +35846,10 @@
         <v>0.5</v>
       </c>
       <c r="D95" s="20" t="s">
-        <v>2631</v>
+        <v>2628</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>2632</v>
+        <v>2629</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>1235</v>
@@ -35763,10 +35884,10 @@
       <c r="V95" s="7"/>
       <c r="W95" s="21"/>
       <c r="X95" s="20" t="s">
-        <v>2633</v>
+        <v>2630</v>
       </c>
       <c r="Y95" s="20" t="s">
-        <v>2634</v>
+        <v>2631</v>
       </c>
       <c r="Z95" s="11" t="s">
         <v>2339</v>
@@ -35985,10 +36106,10 @@
         <v>920</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>919</v>
@@ -36055,10 +36176,10 @@
         <v>2126</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D100" s="11" t="s">
         <v>2125</v>
@@ -36869,10 +36990,10 @@
         <v>2375</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>2374</v>
@@ -37830,7 +37951,7 @@
         <v>368</v>
       </c>
       <c r="E126" s="20" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="F126" s="7" t="s">
         <v>369</v>
@@ -41018,7 +41139,7 @@
         <v>996</v>
       </c>
       <c r="E173" s="20" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="F173" s="7" t="s">
         <v>997</v>
@@ -41152,7 +41273,7 @@
         <v>1900</v>
       </c>
       <c r="E175" s="20" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>1598</v>
@@ -41215,7 +41336,7 @@
         <v>0.5</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="E176" s="11" t="s">
         <v>1139</v>
@@ -41253,10 +41374,10 @@
       <c r="V176" s="7"/>
       <c r="W176" s="7"/>
       <c r="X176" s="20" t="s">
+        <v>2571</v>
+      </c>
+      <c r="Y176" s="20" t="s">
         <v>2572</v>
-      </c>
-      <c r="Y176" s="20" t="s">
-        <v>2573</v>
       </c>
       <c r="Z176" s="11" t="s">
         <v>1148</v>
@@ -41651,7 +41772,7 @@
       <c r="V182" s="7"/>
       <c r="W182" s="7"/>
       <c r="X182" s="20" t="s">
-        <v>2564</v>
+        <v>2654</v>
       </c>
       <c r="Y182" s="20" t="s">
         <v>2563</v>
@@ -41745,10 +41866,10 @@
         <v>0.5</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>2639</v>
+        <v>2636</v>
       </c>
       <c r="E184" s="20" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="F184" s="7" t="s">
         <v>216</v>
@@ -41783,10 +41904,10 @@
       <c r="V184" s="7"/>
       <c r="W184" s="21"/>
       <c r="X184" s="20" t="s">
-        <v>2640</v>
+        <v>2637</v>
       </c>
       <c r="Y184" s="20" t="s">
-        <v>2641</v>
+        <v>2638</v>
       </c>
       <c r="Z184" s="11" t="s">
         <v>224</v>
@@ -41814,7 +41935,7 @@
         <v>2321</v>
       </c>
       <c r="E185" s="20" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="F185" s="7" t="s">
         <v>2322</v>
@@ -42011,7 +42132,7 @@
         <v>0.5</v>
       </c>
       <c r="D188" s="20" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="E188" s="11" t="s">
         <v>1245</v>
@@ -42049,10 +42170,10 @@
       <c r="V188" s="7"/>
       <c r="W188" s="7"/>
       <c r="X188" s="20" t="s">
-        <v>2619</v>
+        <v>2652</v>
       </c>
       <c r="Y188" s="20" t="s">
-        <v>2620</v>
+        <v>2653</v>
       </c>
       <c r="Z188" s="11" t="s">
         <v>1254</v>
@@ -42669,10 +42790,10 @@
         <v>90</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C198" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D198" s="11" t="s">
         <v>86</v>
@@ -42746,7 +42867,7 @@
         <v>807</v>
       </c>
       <c r="E199" s="20" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="F199" s="7" t="s">
         <v>808</v>
@@ -42878,7 +42999,7 @@
         <v>491</v>
       </c>
       <c r="E201" s="20" t="s">
-        <v>2642</v>
+        <v>2639</v>
       </c>
       <c r="F201" s="7" t="s">
         <v>492</v>
@@ -42939,10 +43060,10 @@
         <v>206</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C202" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D202" s="11" t="s">
         <v>202</v>
@@ -44072,7 +44193,7 @@
         <v>390</v>
       </c>
       <c r="E219" s="20" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="F219" s="7" t="s">
         <v>391</v>
@@ -44140,7 +44261,7 @@
         <v>1453</v>
       </c>
       <c r="E220" s="20" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="F220" s="7" t="s">
         <v>1454</v>
@@ -44206,7 +44327,7 @@
         <v>699</v>
       </c>
       <c r="E221" s="20" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="F221" s="7" t="s">
         <v>391</v>
@@ -44342,7 +44463,7 @@
         <v>1860</v>
       </c>
       <c r="E223" s="20" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F223" s="7" t="s">
         <v>1861</v>
@@ -44407,7 +44528,7 @@
         <v>0.7</v>
       </c>
       <c r="D224" s="20" t="s">
-        <v>2643</v>
+        <v>2640</v>
       </c>
       <c r="E224" s="11" t="s">
         <v>1759</v>
@@ -44445,10 +44566,10 @@
       <c r="V224" s="7"/>
       <c r="W224" s="7"/>
       <c r="X224" s="20" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="Y224" s="20" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="Z224" s="11" t="s">
         <v>1765</v>
@@ -44473,7 +44594,7 @@
         <v>0.5</v>
       </c>
       <c r="D225" s="20" t="s">
-        <v>2645</v>
+        <v>2642</v>
       </c>
       <c r="E225" s="11" t="s">
         <v>472</v>
@@ -44511,10 +44632,10 @@
       <c r="V225" s="7"/>
       <c r="W225" s="7"/>
       <c r="X225" s="20" t="s">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="Y225" s="20" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="Z225" s="11" t="s">
         <v>480</v>
@@ -44608,7 +44729,7 @@
         <v>2480</v>
       </c>
       <c r="E227" s="20" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="F227" s="7" t="s">
         <v>2481</v>
@@ -44671,10 +44792,10 @@
         <v>0.5</v>
       </c>
       <c r="D228" s="20" t="s">
-        <v>2635</v>
+        <v>2632</v>
       </c>
       <c r="E228" s="20" t="s">
-        <v>2632</v>
+        <v>2629</v>
       </c>
       <c r="F228" s="7" t="s">
         <v>1235</v>
@@ -44709,10 +44830,10 @@
       <c r="V228" s="7"/>
       <c r="W228" s="21"/>
       <c r="X228" s="20" t="s">
-        <v>2636</v>
+        <v>2633</v>
       </c>
       <c r="Y228" s="20" t="s">
-        <v>2637</v>
+        <v>2634</v>
       </c>
       <c r="Z228" s="11" t="s">
         <v>1243</v>
@@ -44799,10 +44920,10 @@
         <v>988</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="C230" s="17" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="D230" s="11" t="s">
         <v>986</v>
@@ -44959,10 +45080,10 @@
         <v>2559</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>